<commit_message>
edited the content of  BugReport_MQA.xlsx to cause a conflict
</commit_message>
<xml_diff>
--- a/BugReport_MQA.xlsx
+++ b/BugReport_MQA.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>add new words</t>
+  </si>
+  <si>
+    <t>add conflict</t>
   </si>
 </sst>
 </file>
@@ -688,10 +691,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -880,6 +883,11 @@
         <v>34</v>
       </c>
     </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>

</xml_diff>

<commit_message>
appended content to BugReport_MQA.xls
</commit_message>
<xml_diff>
--- a/BugReport_MQA.xlsx
+++ b/BugReport_MQA.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>add new words</t>
+  </si>
+  <si>
+    <t>content to append</t>
   </si>
 </sst>
 </file>
@@ -688,10 +691,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -880,6 +883,11 @@
         <v>34</v>
       </c>
     </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>

</xml_diff>